<commit_message>
add New TC,TS, and latest reports
</commit_message>
<xml_diff>
--- a/Data Files/excel file/Verify Get Single User.xlsx
+++ b/Data Files/excel file/Verify Get Single User.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="15">
   <si>
     <t>apiKey</t>
   </si>
@@ -28,10 +28,16 @@
     <t>remark</t>
   </si>
   <si>
-    <t>Missing API key</t>
+    <t>Missing API key.</t>
   </si>
   <si>
     <t>Check authorization</t>
+  </si>
+  <si>
+    <t>aaaa</t>
+  </si>
+  <si>
+    <t>Invalid API key.</t>
   </si>
   <si>
     <t>reqres-free-v1</t>
@@ -344,30 +350,33 @@
       <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
+      <c r="B3" s="2">
+        <v>1.0</v>
+      </c>
       <c r="C3" s="2">
+        <v>401.0</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="2">
         <v>200.0</v>
       </c>
-      <c r="E3" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="B4" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="C4" s="2">
-        <v>401.0</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>6</v>
+      <c r="E4" s="1" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B5" s="2">
         <v>2.0</v>
@@ -376,12 +385,12 @@
         <v>200.0</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B6" s="1">
         <v>100.0</v>
@@ -390,27 +399,27 @@
         <v>404.0</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C7" s="1">
         <v>404.0</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>